<commit_message>
Test Data is Updated
</commit_message>
<xml_diff>
--- a/src/main/java/com/sa/test/data/TestCases.xlsx
+++ b/src/main/java/com/sa/test/data/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14895" windowHeight="4155" tabRatio="236" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15675" windowHeight="5310" tabRatio="236" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="41" r:id="rId1"/>
@@ -15,11 +15,12 @@
     <definedName name="PartnerCollege">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:F15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="141">
   <si>
     <t>Sr No</t>
   </si>
@@ -439,6 +440,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -919,7 +923,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -965,7 +969,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1029,7 +1033,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
Latest Testdata and TestCases
</commit_message>
<xml_diff>
--- a/src/main/java/com/sa/test/data/TestCases.xlsx
+++ b/src/main/java/com/sa/test/data/TestCases.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15675" windowHeight="5310" tabRatio="236" activeTab="1"/>
+    <workbookView activeTab="1" tabRatio="236" windowHeight="5310" windowWidth="15675" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSuite" sheetId="41" r:id="rId1"/>
-    <sheet name="TestCase" sheetId="40" r:id="rId2"/>
+    <sheet name="TestSuite" r:id="rId1" sheetId="41"/>
+    <sheet name="TestCase" r:id="rId2" sheetId="40"/>
   </sheets>
   <definedNames>
     <definedName name="Degree">#REF!</definedName>
     <definedName name="PartnerCollege">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:F15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="158">
   <si>
     <t>Sr No</t>
   </si>
@@ -439,10 +438,61 @@
     <t>ChangePassword</t>
   </si>
   <si>
+    <t>DeleteElopUser</t>
+  </si>
+  <si>
+    <t>Scenario_T_46</t>
+  </si>
+  <si>
+    <t>Delete Particular row user</t>
+  </si>
+  <si>
+    <t>ElopUserResetPassword</t>
+  </si>
+  <si>
+    <t>Check  weather  the reset password link has been sent to email address</t>
+  </si>
+  <si>
+    <t>Approve PaymentorCredit</t>
+  </si>
+  <si>
+    <t>Scenario_T_47</t>
+  </si>
+  <si>
+    <t>Scenario_T_48</t>
+  </si>
+  <si>
+    <t>Scenario_T_49</t>
+  </si>
+  <si>
+    <t>Scenario_T_50</t>
+  </si>
+  <si>
+    <t>Check wether the payment credit functionality working or not</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
+    <t>DeleteSiteUser</t>
+  </si>
+  <si>
+    <t>Delete unwanted SiteUser</t>
+  </si>
+  <si>
+    <t>SiteUserResetPassword</t>
+  </si>
+  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>ParentInActive</t>
+  </si>
+  <si>
+    <t>Disable the parent whose not paying week payments</t>
+  </si>
+  <si>
+    <t>ParentResetPassword</t>
   </si>
 </sst>
 </file>
@@ -557,52 +607,52 @@
     </border>
   </borders>
   <cellStyleXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="165"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="164"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="5">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -615,14 +665,14 @@
     <cellStyle name="Excel Built-in Normal 3" xfId="11"/>
     <cellStyle name="Heading" xfId="6"/>
     <cellStyle name="Heading1" xfId="7"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="8"/>
     <cellStyle name="Normal 3" xfId="1"/>
     <cellStyle name="Result" xfId="9"/>
     <cellStyle name="Result2" xfId="10"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -639,10 +689,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -798,7 +848,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -807,13 +857,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -823,7 +873,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -832,7 +882,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -841,7 +891,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -851,12 +901,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -887,7 +937,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -906,7 +956,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -922,14 +972,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="C7" pane="bottomLeft" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="83.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -959,29 +1009,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A8" ySplit="1"/>
+      <selection activeCell="H20" pane="bottomLeft" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="71" style="8" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="4" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="8" width="71.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="11.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="6.76171875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1010,7 +1060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1">
+    <row customHeight="1" ht="18.75" r="2" spans="1:8">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1033,10 +1083,10 @@
         <v>10</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="3" spans="1:8">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1058,11 +1108,9 @@
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H3" s="5"/>
+    </row>
+    <row customHeight="1" ht="16.5" r="4" spans="1:8">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1084,16 +1132,14 @@
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="5"/>
+    </row>
+    <row customHeight="1" ht="16.5" r="5" spans="1:8">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>8</v>
@@ -1105,21 +1151,19 @@
         <v>20</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+      <c r="H5" s="5"/>
+    </row>
+    <row customHeight="1" ht="16.5" r="6" spans="1:8">
       <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -1131,18 +1175,19 @@
         <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H6" s="5"/>
+    </row>
+    <row customHeight="1" ht="16.5" r="7" spans="1:8">
       <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>8</v>
@@ -1154,18 +1199,19 @@
         <v>26</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
@@ -1177,18 +1223,21 @@
         <v>28</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" customHeight="1">
+      <c r="H8" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" spans="1:8">
       <c r="A9" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>8</v>
@@ -1200,536 +1249,567 @@
         <v>33</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="10" spans="1:8">
       <c r="A10" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" spans="1:8">
       <c r="A11" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="17.25" r="12" spans="1:8">
       <c r="A12" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="17.25" r="13" spans="1:8">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="14" spans="1:8">
+      <c r="A14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="15" spans="1:8">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="16" spans="1:8">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="9">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="9">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="9">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="G19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="9">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="9">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="9">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="C21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="9">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="G21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="9">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="C22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="9">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="G22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="9">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="C23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="9">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="G23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="9">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="C24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="9">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="G24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="9">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="9">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="G25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="9">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="C26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="9">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="G26" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="9">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="C27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="9">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="G27" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="9">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="C28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="9">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="G28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="9">
+        <v>23</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="C29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="9">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="G29" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="9">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="C30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="9">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="G30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="9">
+        <v>25</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="C31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="9">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="G31" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="9">
+        <v>26</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="C32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="9">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="9">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="9">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="9">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="9">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="9">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="9">
-        <v>31</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>10</v>
@@ -1737,10 +1817,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="9">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>8</v>
@@ -1749,10 +1829,10 @@
         <v>12</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>10</v>
@@ -1760,10 +1840,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="9">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>8</v>
@@ -1772,10 +1852,10 @@
         <v>12</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>10</v>
@@ -1783,10 +1863,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="9">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>8</v>
@@ -1795,10 +1875,10 @@
         <v>12</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>10</v>
@@ -1806,10 +1886,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>8</v>
@@ -1818,7 +1898,7 @@
         <v>12</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>98</v>
@@ -1829,10 +1909,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="9">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>8</v>
@@ -1841,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>98</v>
@@ -1852,10 +1932,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="9">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>8</v>
@@ -1864,10 +1944,10 @@
         <v>12</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>10</v>
@@ -1875,10 +1955,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="9">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>8</v>
@@ -1887,10 +1967,10 @@
         <v>12</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>10</v>
@@ -1898,10 +1978,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="9">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>8</v>
@@ -1910,10 +1990,10 @@
         <v>12</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>10</v>
@@ -1921,10 +2001,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="9">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>8</v>
@@ -1933,10 +2013,10 @@
         <v>12</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>10</v>
@@ -1944,10 +2024,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="9">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>8</v>
@@ -1956,10 +2036,10 @@
         <v>12</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>10</v>
@@ -1967,10 +2047,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="9">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>8</v>
@@ -1979,10 +2059,10 @@
         <v>12</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>10</v>
@@ -1990,10 +2070,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="9">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>8</v>
@@ -2002,10 +2082,10 @@
         <v>12</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>10</v>
@@ -2013,10 +2093,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="9">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>8</v>
@@ -2025,10 +2105,10 @@
         <v>12</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>10</v>
@@ -2036,59 +2116,253 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="9">
+        <v>40</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="9">
+        <v>41</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="9">
+        <v>42</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="9">
+        <v>43</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="9">
+        <v>44</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="9">
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B51" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="9">
+        <v>46</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="9">
+        <v>47</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" s="8" t="s">
+      <c r="C53" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="9"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="9"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="9"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="9"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1">
-      <c r="H51" s="5"/>
+      <c r="G53" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="H54" s="5"/>
+      <c r="A54" s="9">
+        <v>48</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="9">
+        <v>49</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="9">
+        <v>50</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="9">
+        <v>51</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="58" spans="1:8">
+      <c r="A58" s="9">
+        <v>52</v>
+      </c>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="9">
+        <v>55</v>
+      </c>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="9">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>